<commit_message>
Added and verified tonal annoyance weighting option for MATLAB ECMA 418-2 tonality
</commit_message>
<xml_diff>
--- a/validation/ECMA-418-2/reference/verification_ECMA-418-2_2025_LR.xlsx
+++ b/validation/ECMA-418-2/reference/verification_ECMA-418-2_2025_LR.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://testlivesalfordac-my.sharepoint.com/personal/m_j_lotinga_edu_salford_ac_uk/Documents/Code/refmap-psychoacoustics/validation/ECMA-418-2_2022/reference/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m_lot\source\repos\refmap-psychoacoustics\validation\ECMA-418-2\reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="11_8A73D4BC6E2EB011B8B47F0F4295FAA6B348A397" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C32CD327-4C49-4B08-87BE-78B12D583C77}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC94411-6166-4D7E-9943-048CFE1689C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14303" yWindow="-2595" windowWidth="17115" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>Rough_HMS_LR</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>Channel</t>
+  </si>
+  <si>
+    <t>Tonal_Taw_HMS_LR</t>
   </si>
 </sst>
 </file>
@@ -416,15 +419,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:B1"/>
+      <selection activeCell="F4" sqref="F4:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -440,8 +443,11 @@
       <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="F1" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -457,8 +463,11 @@
       <c r="E2">
         <v>1</v>
       </c>
+      <c r="F2">
+        <v>1.03</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -474,8 +483,11 @@
       <c r="E3">
         <v>1.34</v>
       </c>
+      <c r="F3">
+        <v>1.37</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -491,8 +503,11 @@
       <c r="E4">
         <v>0.14299999999999999</v>
       </c>
+      <c r="F4">
+        <v>0.154</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -507,6 +522,9 @@
       </c>
       <c r="E5">
         <v>0.155</v>
+      </c>
+      <c r="F5">
+        <v>0.16700000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>